<commit_message>
Update content in party.html
Add all bridal party names, and organize appearance of placeholder photos.
</commit_message>
<xml_diff>
--- a/documents/Wed_Info.xlsx
+++ b/documents/Wed_Info.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rosa.avalos\Documents\MIS\2017\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexw\Documents\GitHub\alexwarren1989.github.io\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="7995" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13500" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="RSVP" sheetId="2" r:id="rId1"/>

</xml_diff>

<commit_message>
Update content in travel.html
</commit_message>
<xml_diff>
--- a/documents/Wed_Info.xlsx
+++ b/documents/Wed_Info.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rosa.avalos\Documents\MIS\2017\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexw\Documents\GitHub\alexwarren1989.github.io\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="7995" firstSheet="3" activeTab="3"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="RSVP" sheetId="2" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <sheet name="Gifts" sheetId="9" r:id="rId8"/>
     <sheet name="Attire" sheetId="10" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -619,7 +619,7 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection sqref="A1:A20"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>